<commit_message>
258 - Updated leish report export sheet so gender dist is indicated as female dist
</commit_message>
<xml_diff>
--- a/Nada.UI/Exports/Leishmaniasis_Report_Card.xlsx
+++ b/Nada.UI/Exports/Leishmaniasis_Report_Card.xlsx
@@ -460,9 +460,6 @@
 (%, # clinical cases / # new cases)</t>
   </si>
   <si>
-    <t>Gender distribution:</t>
-  </si>
-  <si>
     <r>
       <t>Age group distribution (%, &lt; 5/5-14/</t>
     </r>
@@ -488,6 +485,9 @@
   <si>
     <t>Months elapsed between onset
 of symptoms and diagnosis (median):</t>
+  </si>
+  <si>
+    <t>Gender distribution - female:</t>
   </si>
 </sst>
 </file>
@@ -1186,253 +1186,184 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="31" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="31" fillId="0" borderId="12" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="31" fillId="0" borderId="11" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1441,97 +1372,166 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="11" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="31" fillId="0" borderId="12" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="31" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="77">
@@ -1734,8 +1734,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="245851376"/>
-        <c:axId val="245851760"/>
+        <c:axId val="385055184"/>
+        <c:axId val="385055576"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1822,11 +1822,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="245873688"/>
-        <c:axId val="245873304"/>
+        <c:axId val="187965064"/>
+        <c:axId val="187964672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="245851376"/>
+        <c:axId val="385055184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1846,7 +1846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245851760"/>
+        <c:crossAx val="385055576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1854,7 +1854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245851760"/>
+        <c:axId val="385055576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,12 +1884,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245851376"/>
+        <c:crossAx val="385055184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245873304"/>
+        <c:axId val="187964672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,12 +1918,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245873688"/>
+        <c:crossAx val="187965064"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="245873688"/>
+        <c:axId val="187965064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245873304"/>
+        <c:crossAx val="187964672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2410,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78:N79"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2442,137 +2442,137 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="2:14" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="141" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="64"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="145"/>
     </row>
     <row r="4" spans="2:14" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="120"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
+      <c r="B4" s="151"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
+      <c r="H4" s="150"/>
+      <c r="I4" s="150"/>
+      <c r="J4" s="150"/>
+      <c r="K4" s="150"/>
+      <c r="L4" s="150"/>
+      <c r="M4" s="150"/>
+      <c r="N4" s="150"/>
     </row>
     <row r="5" spans="2:14" s="19" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="97"/>
+      <c r="N5" s="97"/>
     </row>
     <row r="6" spans="2:14" s="20" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="125" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="122"/>
-      <c r="N6" s="122"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
     </row>
     <row r="7" spans="2:14" s="20" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="126"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="125" t="s">
+      <c r="C7" s="93"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
-      <c r="N7" s="128"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="95"/>
     </row>
     <row r="8" spans="2:14" s="21" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="126"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="129" t="s">
+      <c r="C8" s="93"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="130"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="130"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="143"/>
+      <c r="N8" s="143"/>
     </row>
     <row r="9" spans="2:14" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="126"/>
+      <c r="C9" s="93"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="143"/>
+      <c r="N9" s="143"/>
     </row>
     <row r="10" spans="2:14" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
+      <c r="B10" s="148"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="150"/>
+      <c r="G10" s="150"/>
+      <c r="H10" s="150"/>
+      <c r="I10" s="150"/>
       <c r="J10" s="25"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
@@ -2580,238 +2580,238 @@
       <c r="N10" s="26"/>
     </row>
     <row r="11" spans="2:14" s="19" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
     </row>
     <row r="12" spans="2:14" s="27" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="131"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="65" t="s">
+      <c r="B12" s="84"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="65" t="s">
+      <c r="H12" s="147"/>
+      <c r="I12" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="65" t="s">
+      <c r="J12" s="147"/>
+      <c r="K12" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="66"/>
-      <c r="M12" s="65" t="s">
+      <c r="L12" s="147"/>
+      <c r="M12" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="66"/>
+      <c r="N12" s="147"/>
     </row>
     <row r="13" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="67"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="115"/>
     </row>
     <row r="14" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="37"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="119"/>
+      <c r="N14" s="120"/>
     </row>
     <row r="15" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="36" t="s">
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="120"/>
+      <c r="M15" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="37"/>
+      <c r="N15" s="120"/>
     </row>
     <row r="16" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="133" t="s">
+      <c r="B16" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="47" t="s">
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="47" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="N16" s="48"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="48"/>
-    </row>
-    <row r="18" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="75"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="39"/>
     </row>
     <row r="19" spans="2:14" s="27" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="50" t="s">
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="L19" s="67"/>
-      <c r="M19" s="36" t="s">
+      <c r="L19" s="115"/>
+      <c r="M19" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="N19" s="37"/>
+      <c r="N19" s="120"/>
     </row>
     <row r="20" spans="2:14" s="27" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="99"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="121"/>
       <c r="G20" s="30"/>
       <c r="H20" s="31"/>
       <c r="I20" s="32"/>
       <c r="J20" s="31"/>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="37"/>
-      <c r="M20" s="36" t="s">
+      <c r="L20" s="120"/>
+      <c r="M20" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="N20" s="37"/>
+      <c r="N20" s="120"/>
     </row>
     <row r="21" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="47" t="s">
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="48"/>
-      <c r="M21" s="47" t="s">
+      <c r="L21" s="37"/>
+      <c r="M21" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="N21" s="48"/>
+      <c r="N21" s="37"/>
     </row>
     <row r="22" spans="2:14" s="27" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="74" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="L22" s="75"/>
-      <c r="M22" s="74" t="s">
+      <c r="L22" s="39"/>
+      <c r="M22" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="N22" s="75"/>
+      <c r="N22" s="39"/>
     </row>
     <row r="23" spans="2:14" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
@@ -2831,21 +2831,21 @@
       <c r="N23" s="28"/>
     </row>
     <row r="24" spans="2:14" s="27" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
+      <c r="C24" s="158"/>
+      <c r="D24" s="158"/>
+      <c r="E24" s="158"/>
+      <c r="F24" s="158"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="158"/>
+      <c r="K24" s="158"/>
+      <c r="L24" s="158"/>
+      <c r="M24" s="158"/>
+      <c r="N24" s="158"/>
     </row>
     <row r="25" spans="2:14" s="4" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
@@ -2964,58 +2964,58 @@
       <c r="N42" s="8"/>
     </row>
     <row r="43" spans="2:14" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="135" t="s">
+      <c r="B43" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="84"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="84"/>
-      <c r="K43" s="84"/>
-      <c r="L43" s="84"/>
-      <c r="M43" s="84"/>
-      <c r="N43" s="84"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="65"/>
+      <c r="J43" s="65"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
+      <c r="N43" s="65"/>
     </row>
     <row r="44" spans="2:14" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="138" t="s">
+      <c r="B44" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="84"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="84"/>
-      <c r="L44" s="84"/>
-      <c r="M44" s="84"/>
-      <c r="N44" s="84"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="65"/>
+      <c r="M44" s="65"/>
+      <c r="N44" s="65"/>
     </row>
     <row r="45" spans="2:14" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="6"/>
     </row>
     <row r="46" spans="2:14" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="53"/>
-      <c r="M46" s="53"/>
-      <c r="N46" s="53"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
+      <c r="M46" s="83"/>
+      <c r="N46" s="83"/>
     </row>
     <row r="47" spans="2:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3026,97 +3026,97 @@
     <row r="53" spans="2:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:14" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="96" t="s">
+      <c r="B59" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="97"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="97"/>
-      <c r="F59" s="97"/>
-      <c r="G59" s="97"/>
-      <c r="H59" s="97"/>
-      <c r="I59" s="97"/>
-      <c r="J59" s="97"/>
-      <c r="K59" s="97"/>
-      <c r="L59" s="97"/>
-      <c r="M59" s="97"/>
-      <c r="N59" s="97"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="82"/>
+      <c r="M59" s="82"/>
+      <c r="N59" s="82"/>
     </row>
     <row r="60" spans="2:14" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="148" t="s">
+      <c r="B60" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C60" s="149"/>
-      <c r="D60" s="149"/>
-      <c r="E60" s="149"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="150" t="s">
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="122"/>
+      <c r="H60" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="I60" s="151"/>
-      <c r="J60" s="152"/>
-      <c r="K60" s="153"/>
-      <c r="L60" s="153"/>
-      <c r="M60" s="153"/>
-      <c r="N60" s="153"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="61"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="62"/>
     </row>
     <row r="61" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C61" s="112"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="112"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="111" t="s">
+      <c r="C61" s="74"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="122"/>
+      <c r="H61" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I61" s="111"/>
-      <c r="J61" s="111"/>
-      <c r="K61" s="111"/>
-      <c r="L61" s="111"/>
-      <c r="M61" s="55"/>
-      <c r="N61" s="55"/>
+      <c r="I61" s="40"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="40"/>
+      <c r="L61" s="40"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="41"/>
     </row>
     <row r="62" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="111" t="s">
+      <c r="B62" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C62" s="111"/>
-      <c r="D62" s="111"/>
-      <c r="E62" s="111"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="111" t="s">
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I62" s="112"/>
-      <c r="J62" s="112"/>
-      <c r="K62" s="112"/>
-      <c r="L62" s="112"/>
-      <c r="M62" s="55"/>
-      <c r="N62" s="55"/>
+      <c r="I62" s="74"/>
+      <c r="J62" s="74"/>
+      <c r="K62" s="74"/>
+      <c r="L62" s="74"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
     </row>
     <row r="63" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="139" t="s">
+      <c r="B63" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="139"/>
-      <c r="D63" s="139"/>
-      <c r="E63" s="139"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="111" t="s">
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="41"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="I63" s="112"/>
-      <c r="J63" s="112"/>
-      <c r="K63" s="112"/>
-      <c r="L63" s="112"/>
-      <c r="M63" s="55"/>
-      <c r="N63" s="55"/>
+      <c r="I63" s="74"/>
+      <c r="J63" s="74"/>
+      <c r="K63" s="74"/>
+      <c r="L63" s="74"/>
+      <c r="M63" s="41"/>
+      <c r="N63" s="41"/>
     </row>
     <row r="64" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
@@ -3134,608 +3134,542 @@
       <c r="N64" s="15"/>
     </row>
     <row r="65" spans="2:14" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="96" t="s">
+      <c r="B65" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="97"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="97"/>
-      <c r="F65" s="97"/>
-      <c r="G65" s="97"/>
-      <c r="H65" s="97"/>
-      <c r="I65" s="97"/>
-      <c r="J65" s="97"/>
-      <c r="K65" s="97"/>
-      <c r="L65" s="97"/>
-      <c r="M65" s="97"/>
-      <c r="N65" s="97"/>
+      <c r="C65" s="82"/>
+      <c r="D65" s="82"/>
+      <c r="E65" s="82"/>
+      <c r="F65" s="82"/>
+      <c r="G65" s="82"/>
+      <c r="H65" s="82"/>
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="82"/>
+      <c r="N65" s="82"/>
     </row>
     <row r="66" spans="2:14" s="4" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="100"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="94" t="s">
+      <c r="B66" s="123"/>
+      <c r="C66" s="123"/>
+      <c r="D66" s="123"/>
+      <c r="E66" s="123"/>
+      <c r="F66" s="123"/>
+      <c r="G66" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="95"/>
-      <c r="I66" s="94" t="s">
+      <c r="H66" s="46"/>
+      <c r="I66" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J66" s="95"/>
-      <c r="K66" s="94" t="s">
+      <c r="J66" s="46"/>
+      <c r="K66" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="L66" s="95"/>
-      <c r="M66" s="94" t="s">
+      <c r="L66" s="46"/>
+      <c r="M66" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="N66" s="95"/>
+      <c r="N66" s="46"/>
     </row>
     <row r="67" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="142" t="s">
+      <c r="B67" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="143"/>
-      <c r="D67" s="143"/>
-      <c r="E67" s="143"/>
-      <c r="F67" s="143"/>
-      <c r="G67" s="144"/>
-      <c r="H67" s="145"/>
-      <c r="I67" s="144"/>
-      <c r="J67" s="145"/>
-      <c r="K67" s="144"/>
-      <c r="L67" s="145"/>
-      <c r="M67" s="146" t="s">
+      <c r="C67" s="79"/>
+      <c r="D67" s="79"/>
+      <c r="E67" s="79"/>
+      <c r="F67" s="79"/>
+      <c r="G67" s="80"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="80"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="80"/>
+      <c r="L67" s="53"/>
+      <c r="M67" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="N67" s="145"/>
+      <c r="N67" s="53"/>
     </row>
     <row r="68" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="91" t="s">
+      <c r="B68" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="92"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="92"/>
-      <c r="G68" s="113"/>
-      <c r="H68" s="114"/>
-      <c r="I68" s="113"/>
-      <c r="J68" s="114"/>
-      <c r="K68" s="113"/>
-      <c r="L68" s="114"/>
-      <c r="M68" s="156" t="s">
+      <c r="C68" s="114"/>
+      <c r="D68" s="114"/>
+      <c r="E68" s="114"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="48"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="48"/>
+      <c r="M68" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="N68" s="114"/>
+      <c r="N68" s="48"/>
     </row>
     <row r="69" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="93" t="s">
+      <c r="B69" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="93"/>
-      <c r="D69" s="93"/>
-      <c r="E69" s="93"/>
-      <c r="F69" s="93"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="50"/>
-      <c r="I69" s="51" t="s">
+      <c r="C69" s="110"/>
+      <c r="D69" s="110"/>
+      <c r="E69" s="110"/>
+      <c r="F69" s="110"/>
+      <c r="G69" s="111"/>
+      <c r="H69" s="112"/>
+      <c r="I69" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="J69" s="52"/>
-      <c r="K69" s="51" t="s">
+      <c r="J69" s="55"/>
+      <c r="K69" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L69" s="52"/>
-      <c r="M69" s="51" t="s">
+      <c r="L69" s="55"/>
+      <c r="M69" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="N69" s="52"/>
+      <c r="N69" s="55"/>
     </row>
     <row r="70" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="38" t="s">
+      <c r="B70" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="C70" s="38"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="155"/>
-      <c r="H70" s="155"/>
-      <c r="I70" s="39" t="s">
+      <c r="C70" s="153"/>
+      <c r="D70" s="153"/>
+      <c r="E70" s="153"/>
+      <c r="F70" s="153"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="J70" s="40"/>
-      <c r="K70" s="39" t="s">
+      <c r="J70" s="155"/>
+      <c r="K70" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="L70" s="40"/>
-      <c r="M70" s="39" t="s">
+      <c r="L70" s="155"/>
+      <c r="M70" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="N70" s="40"/>
+      <c r="N70" s="155"/>
     </row>
     <row r="71" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="93" t="s">
+      <c r="B71" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="C71" s="93"/>
-      <c r="D71" s="93"/>
-      <c r="E71" s="93"/>
-      <c r="F71" s="93"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="50"/>
-      <c r="I71" s="50"/>
-      <c r="J71" s="50"/>
-      <c r="K71" s="76" t="s">
+      <c r="C71" s="110"/>
+      <c r="D71" s="110"/>
+      <c r="E71" s="110"/>
+      <c r="F71" s="110"/>
+      <c r="G71" s="111"/>
+      <c r="H71" s="112"/>
+      <c r="I71" s="112"/>
+      <c r="J71" s="112"/>
+      <c r="K71" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="L71" s="77"/>
-      <c r="M71" s="76" t="s">
+      <c r="L71" s="129"/>
+      <c r="M71" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="N71" s="77"/>
+      <c r="N71" s="129"/>
     </row>
     <row r="72" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="38" t="s">
+      <c r="B72" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="155"/>
-      <c r="H72" s="155"/>
-      <c r="I72" s="155"/>
-      <c r="J72" s="155"/>
-      <c r="K72" s="39" t="s">
+      <c r="C72" s="153"/>
+      <c r="D72" s="153"/>
+      <c r="E72" s="153"/>
+      <c r="F72" s="153"/>
+      <c r="G72" s="42"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="42"/>
+      <c r="J72" s="42"/>
+      <c r="K72" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="L72" s="40"/>
-      <c r="M72" s="39" t="s">
+      <c r="L72" s="155"/>
+      <c r="M72" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="N72" s="40"/>
+      <c r="N72" s="155"/>
     </row>
     <row r="73" spans="2:14" s="27" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="78" t="s">
+      <c r="B73" s="130" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="78"/>
-      <c r="D73" s="78"/>
-      <c r="E73" s="78"/>
-      <c r="F73" s="78"/>
-      <c r="G73" s="79"/>
-      <c r="H73" s="80"/>
-      <c r="I73" s="79"/>
-      <c r="J73" s="80"/>
-      <c r="K73" s="79" t="s">
+      <c r="C73" s="130"/>
+      <c r="D73" s="130"/>
+      <c r="E73" s="130"/>
+      <c r="F73" s="130"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="43"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="L73" s="80"/>
-      <c r="M73" s="79" t="s">
+      <c r="L73" s="44"/>
+      <c r="M73" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="N73" s="80"/>
+      <c r="N73" s="44"/>
     </row>
     <row r="74" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="140" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="141"/>
-      <c r="D74" s="141"/>
-      <c r="E74" s="141"/>
-      <c r="F74" s="141"/>
-      <c r="G74" s="89"/>
-      <c r="H74" s="90"/>
-      <c r="I74" s="89"/>
-      <c r="J74" s="90"/>
-      <c r="K74" s="89" t="s">
+      <c r="B74" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" s="77"/>
+      <c r="D74" s="77"/>
+      <c r="E74" s="77"/>
+      <c r="F74" s="77"/>
+      <c r="G74" s="138"/>
+      <c r="H74" s="139"/>
+      <c r="I74" s="138"/>
+      <c r="J74" s="139"/>
+      <c r="K74" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="L74" s="90"/>
-      <c r="M74" s="89" t="s">
+      <c r="L74" s="139"/>
+      <c r="M74" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="N74" s="90"/>
+      <c r="N74" s="139"/>
     </row>
     <row r="75" spans="2:14" s="27" customFormat="1" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42"/>
-      <c r="F75" s="42"/>
-      <c r="G75" s="79"/>
-      <c r="H75" s="80"/>
-      <c r="I75" s="43" t="s">
+      <c r="C75" s="157"/>
+      <c r="D75" s="157"/>
+      <c r="E75" s="157"/>
+      <c r="F75" s="157"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="J75" s="44"/>
-      <c r="K75" s="79" t="s">
+      <c r="J75" s="118"/>
+      <c r="K75" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="L75" s="80"/>
-      <c r="M75" s="43" t="s">
+      <c r="L75" s="44"/>
+      <c r="M75" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="N75" s="44"/>
+      <c r="N75" s="118"/>
     </row>
     <row r="76" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="147" t="s">
+      <c r="B76" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C76" s="147"/>
-      <c r="D76" s="147"/>
-      <c r="E76" s="147"/>
-      <c r="F76" s="147"/>
-      <c r="G76" s="147"/>
-      <c r="H76" s="147"/>
-      <c r="I76" s="147"/>
-      <c r="J76" s="147"/>
-      <c r="K76" s="147"/>
-      <c r="L76" s="147"/>
-      <c r="M76" s="147"/>
-      <c r="N76" s="147"/>
+      <c r="C76" s="56"/>
+      <c r="D76" s="56"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="56"/>
+      <c r="H76" s="56"/>
+      <c r="I76" s="56"/>
+      <c r="J76" s="56"/>
+      <c r="K76" s="56"/>
+      <c r="L76" s="56"/>
+      <c r="M76" s="56"/>
+      <c r="N76" s="56"/>
     </row>
     <row r="77" spans="2:14" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="70" t="s">
+      <c r="B77" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="71"/>
-      <c r="D77" s="71"/>
-      <c r="E77" s="71"/>
-      <c r="F77" s="71"/>
-      <c r="G77" s="71"/>
-      <c r="H77" s="71"/>
-      <c r="I77" s="71"/>
-      <c r="J77" s="71"/>
-      <c r="K77" s="71"/>
-      <c r="L77" s="71"/>
-      <c r="M77" s="71"/>
-      <c r="N77" s="71"/>
+      <c r="C77" s="127"/>
+      <c r="D77" s="127"/>
+      <c r="E77" s="127"/>
+      <c r="F77" s="127"/>
+      <c r="G77" s="127"/>
+      <c r="H77" s="127"/>
+      <c r="I77" s="127"/>
+      <c r="J77" s="127"/>
+      <c r="K77" s="127"/>
+      <c r="L77" s="127"/>
+      <c r="M77" s="127"/>
+      <c r="N77" s="127"/>
     </row>
     <row r="78" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="105" t="s">
+      <c r="B78" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="C78" s="106"/>
-      <c r="D78" s="106"/>
-      <c r="E78" s="106"/>
-      <c r="F78" s="106"/>
-      <c r="G78" s="106"/>
-      <c r="H78" s="106"/>
-      <c r="I78" s="81"/>
-      <c r="J78" s="81"/>
-      <c r="K78" s="81"/>
-      <c r="L78" s="81"/>
-      <c r="M78" s="81"/>
-      <c r="N78" s="81"/>
+      <c r="C78" s="105"/>
+      <c r="D78" s="105"/>
+      <c r="E78" s="105"/>
+      <c r="F78" s="105"/>
+      <c r="G78" s="105"/>
+      <c r="H78" s="105"/>
+      <c r="I78" s="131"/>
+      <c r="J78" s="131"/>
+      <c r="K78" s="131"/>
+      <c r="L78" s="131"/>
+      <c r="M78" s="131"/>
+      <c r="N78" s="131"/>
     </row>
     <row r="79" spans="2:14" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="105" t="s">
+      <c r="B79" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C79" s="107"/>
-      <c r="D79" s="107"/>
-      <c r="E79" s="107"/>
-      <c r="F79" s="107"/>
-      <c r="G79" s="107"/>
-      <c r="H79" s="107"/>
-      <c r="I79" s="81"/>
-      <c r="J79" s="82"/>
-      <c r="K79" s="82"/>
-      <c r="L79" s="82"/>
-      <c r="M79" s="82"/>
-      <c r="N79" s="82"/>
+      <c r="C79" s="106"/>
+      <c r="D79" s="106"/>
+      <c r="E79" s="106"/>
+      <c r="F79" s="106"/>
+      <c r="G79" s="106"/>
+      <c r="H79" s="106"/>
+      <c r="I79" s="131"/>
+      <c r="J79" s="132"/>
+      <c r="K79" s="132"/>
+      <c r="L79" s="132"/>
+      <c r="M79" s="132"/>
+      <c r="N79" s="132"/>
     </row>
     <row r="80" spans="2:14" s="4" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="83"/>
-      <c r="C80" s="84"/>
-      <c r="D80" s="84"/>
-      <c r="E80" s="84"/>
-      <c r="F80" s="84"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="84"/>
-      <c r="J80" s="84"/>
-      <c r="K80" s="84"/>
-      <c r="L80" s="84"/>
-      <c r="M80" s="84"/>
-      <c r="N80" s="84"/>
+      <c r="B80" s="133"/>
+      <c r="C80" s="65"/>
+      <c r="D80" s="65"/>
+      <c r="E80" s="65"/>
+      <c r="F80" s="65"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
+      <c r="J80" s="65"/>
+      <c r="K80" s="65"/>
+      <c r="L80" s="65"/>
+      <c r="M80" s="65"/>
+      <c r="N80" s="65"/>
     </row>
     <row r="81" spans="2:14" s="27" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="86" t="s">
+      <c r="B81" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C81" s="87"/>
-      <c r="D81" s="88"/>
-      <c r="E81" s="88"/>
-      <c r="F81" s="88"/>
-      <c r="G81" s="157" t="s">
+      <c r="C81" s="136"/>
+      <c r="D81" s="137"/>
+      <c r="E81" s="137"/>
+      <c r="F81" s="137"/>
+      <c r="G81" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H81" s="158"/>
-      <c r="I81" s="157" t="s">
+      <c r="H81" s="51"/>
+      <c r="I81" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J81" s="158"/>
+      <c r="J81" s="51"/>
     </row>
     <row r="82" spans="2:14" s="27" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="108" t="s">
+      <c r="B82" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="C82" s="108"/>
-      <c r="D82" s="108"/>
-      <c r="E82" s="108"/>
-      <c r="F82" s="108"/>
-      <c r="G82" s="109"/>
-      <c r="H82" s="109"/>
-      <c r="I82" s="110"/>
-      <c r="J82" s="110"/>
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
+      <c r="E82" s="107"/>
+      <c r="F82" s="107"/>
+      <c r="G82" s="108"/>
+      <c r="H82" s="108"/>
+      <c r="I82" s="109"/>
+      <c r="J82" s="109"/>
     </row>
     <row r="83" spans="2:14" s="27" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="85" t="s">
+      <c r="B83" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="C83" s="85"/>
-      <c r="D83" s="85"/>
-      <c r="E83" s="85"/>
-      <c r="F83" s="85"/>
-      <c r="G83" s="154"/>
-      <c r="H83" s="154"/>
-      <c r="I83" s="154"/>
-      <c r="J83" s="154"/>
+      <c r="C83" s="134"/>
+      <c r="D83" s="134"/>
+      <c r="E83" s="134"/>
+      <c r="F83" s="134"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="63"/>
+      <c r="I83" s="63"/>
+      <c r="J83" s="63"/>
     </row>
     <row r="84" spans="2:14" s="27" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="101" t="s">
+      <c r="B84" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="102"/>
-      <c r="D84" s="102"/>
-      <c r="E84" s="102"/>
-      <c r="F84" s="102"/>
-      <c r="G84" s="103"/>
-      <c r="H84" s="104"/>
-      <c r="I84" s="103"/>
-      <c r="J84" s="104"/>
+      <c r="C84" s="89"/>
+      <c r="D84" s="89"/>
+      <c r="E84" s="89"/>
+      <c r="F84" s="89"/>
+      <c r="G84" s="34"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="34"/>
+      <c r="J84" s="35"/>
     </row>
     <row r="85" spans="2:14" s="27" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="136" t="s">
+      <c r="B85" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C85" s="137"/>
-      <c r="D85" s="137"/>
-      <c r="E85" s="137"/>
-      <c r="F85" s="137"/>
-      <c r="G85" s="47"/>
-      <c r="H85" s="48"/>
-      <c r="I85" s="47"/>
-      <c r="J85" s="48"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="71"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="36"/>
+      <c r="J85" s="37"/>
     </row>
     <row r="86" spans="2:14" s="27" customFormat="1" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="45" t="s">
+      <c r="B86" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C86" s="46"/>
-      <c r="D86" s="46"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="47"/>
-      <c r="H86" s="48"/>
-      <c r="I86" s="47"/>
-      <c r="J86" s="48"/>
+      <c r="C86" s="67"/>
+      <c r="D86" s="67"/>
+      <c r="E86" s="67"/>
+      <c r="F86" s="67"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="37"/>
     </row>
     <row r="87" spans="2:14" s="27" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="68" t="s">
+      <c r="B87" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="C87" s="68"/>
-      <c r="D87" s="68"/>
-      <c r="E87" s="68"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="69"/>
-      <c r="H87" s="69"/>
-      <c r="I87" s="69"/>
-      <c r="J87" s="69"/>
+      <c r="C87" s="124"/>
+      <c r="D87" s="124"/>
+      <c r="E87" s="124"/>
+      <c r="F87" s="124"/>
+      <c r="G87" s="125"/>
+      <c r="H87" s="125"/>
+      <c r="I87" s="125"/>
+      <c r="J87" s="125"/>
     </row>
     <row r="88" spans="2:14" s="27" customFormat="1" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="72" t="s">
+      <c r="B88" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C88" s="73"/>
-      <c r="D88" s="73"/>
-      <c r="E88" s="73"/>
-      <c r="F88" s="73"/>
-      <c r="G88" s="74"/>
-      <c r="H88" s="75"/>
-      <c r="I88" s="74"/>
-      <c r="J88" s="75"/>
+      <c r="C88" s="69"/>
+      <c r="D88" s="69"/>
+      <c r="E88" s="69"/>
+      <c r="F88" s="69"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="39"/>
     </row>
     <row r="89" spans="2:14" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="34" t="s">
+      <c r="B89" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="35"/>
-      <c r="I89" s="35"/>
-      <c r="J89" s="35"/>
-      <c r="K89" s="35"/>
-      <c r="L89" s="35"/>
-      <c r="M89" s="35"/>
+      <c r="C89" s="72"/>
+      <c r="D89" s="72"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="152"/>
+      <c r="G89" s="152"/>
+      <c r="H89" s="152"/>
+      <c r="I89" s="152"/>
+      <c r="J89" s="152"/>
+      <c r="K89" s="152"/>
+      <c r="L89" s="152"/>
+      <c r="M89" s="152"/>
       <c r="N89" s="29"/>
     </row>
     <row r="90" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="34" t="s">
+      <c r="B90" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="35"/>
-      <c r="I90" s="35"/>
-      <c r="J90" s="35"/>
-      <c r="K90" s="35"/>
-      <c r="L90" s="35"/>
-      <c r="M90" s="35"/>
+      <c r="C90" s="72"/>
+      <c r="D90" s="72"/>
+      <c r="E90" s="72"/>
+      <c r="F90" s="152"/>
+      <c r="G90" s="152"/>
+      <c r="H90" s="152"/>
+      <c r="I90" s="152"/>
+      <c r="J90" s="152"/>
+      <c r="K90" s="152"/>
+      <c r="L90" s="152"/>
+      <c r="M90" s="152"/>
     </row>
     <row r="91" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="34" t="s">
+      <c r="B91" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="35"/>
-      <c r="I91" s="35"/>
-      <c r="J91" s="35"/>
-      <c r="K91" s="35"/>
-      <c r="L91" s="35"/>
-      <c r="M91" s="35"/>
+      <c r="C91" s="72"/>
+      <c r="D91" s="72"/>
+      <c r="E91" s="72"/>
+      <c r="F91" s="152"/>
+      <c r="G91" s="152"/>
+      <c r="H91" s="152"/>
+      <c r="I91" s="152"/>
+      <c r="J91" s="152"/>
+      <c r="K91" s="152"/>
+      <c r="L91" s="152"/>
+      <c r="M91" s="152"/>
     </row>
     <row r="92" spans="2:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="34" t="s">
+      <c r="B92" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="34"/>
-      <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="35"/>
-      <c r="I92" s="35"/>
-      <c r="J92" s="35"/>
-      <c r="K92" s="35"/>
-      <c r="L92" s="35"/>
-      <c r="M92" s="35"/>
+      <c r="C92" s="72"/>
+      <c r="D92" s="72"/>
+      <c r="E92" s="72"/>
+      <c r="F92" s="152"/>
+      <c r="G92" s="152"/>
+      <c r="H92" s="152"/>
+      <c r="I92" s="152"/>
+      <c r="J92" s="152"/>
+      <c r="K92" s="152"/>
+      <c r="L92" s="152"/>
+      <c r="M92" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="186">
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="I86:J86"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="H61:L61"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M68:N68"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="M67:N67"/>
-    <mergeCell ref="M69:N69"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="B76:N76"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:N60"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="B43:N43"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B90:E90"/>
-    <mergeCell ref="B91:E91"/>
-    <mergeCell ref="B44:J44"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="H63:L63"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="B59:N59"/>
-    <mergeCell ref="B46:N46"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="B11:N11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="B78:H78"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H62:L62"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="B65:N65"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B89:E89"/>
+    <mergeCell ref="F89:M89"/>
+    <mergeCell ref="F90:M90"/>
+    <mergeCell ref="F91:M91"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="F92:M92"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K8:L9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B87:F87"/>
     <mergeCell ref="G87:H87"/>
     <mergeCell ref="I87:J87"/>
@@ -3760,54 +3694,120 @@
     <mergeCell ref="B84:F84"/>
     <mergeCell ref="G84:H84"/>
     <mergeCell ref="I78:N78"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K8:L9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B89:E89"/>
-    <mergeCell ref="F89:M89"/>
-    <mergeCell ref="F90:M90"/>
-    <mergeCell ref="F91:M91"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="F92:M92"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="B24:N24"/>
-    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="B65:N65"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="B91:E91"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="H63:L63"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="B59:N59"/>
+    <mergeCell ref="B46:N46"/>
+    <mergeCell ref="B78:H78"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="J60:N60"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="B43:N43"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="H62:L62"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="H61:L61"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="B76:N76"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>

</xml_diff>